<commit_message>
Working on NOT NULL constraint
</commit_message>
<xml_diff>
--- a/data-raw/BeatlesSchema.xlsx
+++ b/data-raw/BeatlesSchema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/PFUPipelineTools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D4D811-9C08-1247-B561-808B2D843406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230552BC-56D4-BC4C-9FAE-1249EDB339FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11320" yWindow="760" windowWidth="18920" windowHeight="16440" activeTab="4" xr2:uid="{8A3A5368-3B53-8E41-9868-764DDCC0B41C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>Table</t>
   </si>
@@ -57,9 +57,6 @@
     <t>fk.colname</t>
   </si>
   <si>
-    <t>Member_ID</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -72,15 +69,9 @@
     <t>text</t>
   </si>
   <si>
-    <t>Role_ID</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
-    <t>Tour_ID</t>
-  </si>
-  <si>
     <t>Tour</t>
   </si>
   <si>
@@ -132,7 +123,22 @@
     <t>Both are useful for testing.</t>
   </si>
   <si>
-    <t>TourAge_ID</t>
+    <t>MemberRole</t>
+  </si>
+  <si>
+    <t>MemberID</t>
+  </si>
+  <si>
+    <t>RoleID</t>
+  </si>
+  <si>
+    <t>TourID</t>
+  </si>
+  <si>
+    <t>MemberRoleID</t>
+  </si>
+  <si>
+    <t>TourAgeID</t>
   </si>
 </sst>
 </file>
@@ -525,17 +531,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -545,13 +551,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2201C18E-68FF-424A-961D-99A35BDADC5C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -572,172 +581,223 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" t="s">
-        <v>7</v>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -750,18 +810,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA2AB34-7206-224A-936F-CB3E9B329582}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -769,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -777,7 +835,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -785,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -793,7 +851,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -806,18 +864,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624D293C-7F24-A040-82CD-0CADE7371A84}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -825,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -833,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -841,7 +897,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -849,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -862,17 +918,17 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -880,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -888,7 +944,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -896,7 +952,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on new structure for schema Excel file
</commit_message>
<xml_diff>
--- a/data-raw/BeatlesSchema.xlsx
+++ b/data-raw/BeatlesSchema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/PFUPipelineTools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D66B74-2BC8-6A46-AE1F-8FA450D81D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BF0B13-D31B-B747-AEF8-B4BAABDABE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11320" yWindow="760" windowWidth="18920" windowHeight="16440" activeTab="1" xr2:uid="{8A3A5368-3B53-8E41-9868-764DDCC0B41C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Table</t>
   </si>
@@ -113,7 +113,7 @@
     <t>RoleID</t>
   </si>
   <si>
-    <t>MemberRoleID</t>
+    <t>IsPK</t>
   </si>
 </sst>
 </file>
@@ -526,19 +526,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2201C18E-68FF-424A-961D-99A35BDADC5C}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,131 +547,135 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
       <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
       <c r="E7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F7" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>